<commit_message>
[ISP-2]Configurazione forecast per Intesa
</commit_message>
<xml_diff>
--- a/forcaster-ATM/forcaster-ATM-app/src/baf-configuration/08_Action.xlsx
+++ b/forcaster-ATM/forcaster-ATM-app/src/baf-configuration/08_Action.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="1000" activeTab="2"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" tabRatio="1000"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="1" r:id="rId1"/>
@@ -5177,15 +5177,15 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B44" sqref="B44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="3" width="64.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="35" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="55" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="129.7109375" style="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -5393,7 +5393,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>21</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>21</v>
       </c>
@@ -5884,7 +5884,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>21</v>
       </c>
@@ -5969,7 +5969,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>21</v>
       </c>
@@ -6020,7 +6020,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" ht="15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>21</v>
       </c>
@@ -6175,10 +6175,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:E58">
-    <filterColumn colId="1">
+    <filterColumn colId="3">
       <filters>
-        <filter val="Schedule KPI on objects in current aggr Prelievo"/>
-        <filter val="Schedule KPI on objects in current aggr Versamento"/>
+        <filter val="[Wizard Editor] Wizard Execution On Instance"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -6298,7 +6297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
@@ -9142,6 +9141,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100B88BEDE3A7878C4B83DDF76392E4AF43" ma:contentTypeVersion="0" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="3c9c3c33ec171c11194a64c89f5a23db">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="85f92fa7f7bbf34a5eeb9e781f8a7e8d">
     <xsd:element name="properties">
@@ -9255,12 +9260,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -9271,6 +9270,21 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E742C650-7594-421F-B32B-CC8DCB6B27D0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70487C6D-DF5B-4B20-AFCC-FDCCFD91570A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -9286,21 +9300,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E742C650-7594-421F-B32B-CC8DCB6B27D0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0704EC93-251E-40AE-95F0-F439BA5545C0}">
   <ds:schemaRefs>

</xml_diff>